<commit_message>
fixed ui changes in sec2.2
</commit_message>
<xml_diff>
--- a/Audit_Code/public/ISO_SEC_2_2.xlsx
+++ b/Audit_Code/public/ISO_SEC_2_2.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97154\Desktop\New folder\Active\GRC Abdullah\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ab\Desktop\Compliance\Audit_Code\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB72E71C-10F0-448C-9270-E79358149B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4F8F09D6-5F60-42F8-99ED-B1D29E69C15F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="275">
   <si>
     <t>Context of the organization</t>
   </si>
@@ -269,9 +268,6 @@
     <t>7.4-d</t>
   </si>
   <si>
-    <t>General actions to address risks and opportunities</t>
-  </si>
-  <si>
     <t>6.1.1-a</t>
   </si>
   <si>
@@ -308,9 +304,6 @@
     <t>6.1.2-e-1</t>
   </si>
   <si>
-    <t>Actions in Information security risk assessment to address risks and opportunities</t>
-  </si>
-  <si>
     <t>6.1.3-a</t>
   </si>
   <si>
@@ -329,15 +322,6 @@
     <t>6.1.3-f</t>
   </si>
   <si>
-    <t xml:space="preserve">Actions in Information security risk treatment to address identified risks </t>
-  </si>
-  <si>
-    <t>Actions in Information security risk treatment to address identified risks</t>
-  </si>
-  <si>
-    <t>General Documented Information</t>
-  </si>
-  <si>
     <t>7.5.2-a</t>
   </si>
   <si>
@@ -347,9 +331,6 @@
     <t>7.5.2-c</t>
   </si>
   <si>
-    <t>Documented Information Management: Creation and Updates</t>
-  </si>
-  <si>
     <t>7.5.3-a</t>
   </si>
   <si>
@@ -368,9 +349,6 @@
     <t>7.5.3-f</t>
   </si>
   <si>
-    <t>Control of documented information</t>
-  </si>
-  <si>
     <t>Operation</t>
   </si>
   <si>
@@ -425,12 +403,6 @@
     <t>9.2.1-b</t>
   </si>
   <si>
-    <t>General Internal Audit</t>
-  </si>
-  <si>
-    <t>Internal audit programme</t>
-  </si>
-  <si>
     <t>9.2.2-a</t>
   </si>
   <si>
@@ -440,12 +412,6 @@
     <t>9.2.2-c</t>
   </si>
   <si>
-    <t>General management review</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Management review inputs</t>
-  </si>
-  <si>
     <t>9.3.2-a</t>
   </si>
   <si>
@@ -474,9 +440,6 @@
   </si>
   <si>
     <t>9.3.2-g</t>
-  </si>
-  <si>
-    <t>Management review results</t>
   </si>
   <si>
     <t>Improvement</t>
@@ -894,11 +857,47 @@
   <si>
     <t>9.3.3</t>
   </si>
+  <si>
+    <t>6.1 General actions to address risks and opportunities</t>
+  </si>
+  <si>
+    <t>6.1 Actions in Information security risk assessment to address risks and opportunities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.1 Actions in Information security risk treatment to address identified risks </t>
+  </si>
+  <si>
+    <t>6.1 Actions in Information security risk treatment to address identified risks</t>
+  </si>
+  <si>
+    <t>7.5 General Documented Information</t>
+  </si>
+  <si>
+    <t>7.5 Documented Information Management: Creation and Updates</t>
+  </si>
+  <si>
+    <t>7.5 Control of documented information</t>
+  </si>
+  <si>
+    <t>9.2 General Internal Audit</t>
+  </si>
+  <si>
+    <t>9.2 Internal audit programme</t>
+  </si>
+  <si>
+    <t>9.3 General management review</t>
+  </si>
+  <si>
+    <t>9.3 Management review inputs</t>
+  </si>
+  <si>
+    <t>9.3 Management review results</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1304,12 +1303,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B4EE03-C897-41D0-AEA6-E317B8297387}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B116" sqref="B116"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1500,7 +1499,7 @@
         <v>27</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -1551,7 +1550,7 @@
         <v>30</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -1568,7 +1567,7 @@
         <v>31</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -1585,7 +1584,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -1602,7 +1601,7 @@
         <v>36</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -1619,7 +1618,7 @@
         <v>37</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -1636,7 +1635,7 @@
         <v>38</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1653,7 +1652,7 @@
         <v>39</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1670,7 +1669,7 @@
         <v>40</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1687,7 +1686,7 @@
         <v>41</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -1704,7 +1703,7 @@
         <v>42</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -1721,7 +1720,7 @@
         <v>44</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -1735,10 +1734,10 @@
         <v>43</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -1749,13 +1748,13 @@
         <v>45</v>
       </c>
       <c r="C26" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="E26" s="7" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -1766,13 +1765,13 @@
         <v>45</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>76</v>
+        <v>263</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -1783,13 +1782,13 @@
         <v>45</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>76</v>
+        <v>263</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -1800,13 +1799,13 @@
         <v>45</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>76</v>
+        <v>263</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -1817,13 +1816,13 @@
         <v>45</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>76</v>
+        <v>263</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -1834,13 +1833,13 @@
         <v>45</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>76</v>
+        <v>263</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="51" x14ac:dyDescent="0.25">
@@ -1851,13 +1850,13 @@
         <v>45</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>89</v>
+        <v>264</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -1868,13 +1867,13 @@
         <v>45</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>89</v>
+        <v>264</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="51" x14ac:dyDescent="0.25">
@@ -1885,13 +1884,13 @@
         <v>45</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>89</v>
+        <v>264</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="51" x14ac:dyDescent="0.25">
@@ -1902,13 +1901,13 @@
         <v>45</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>89</v>
+        <v>264</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -1919,13 +1918,13 @@
         <v>45</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>89</v>
+        <v>264</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -1936,13 +1935,13 @@
         <v>45</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>89</v>
+        <v>264</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -1953,13 +1952,13 @@
         <v>45</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>89</v>
+        <v>264</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -1970,13 +1969,13 @@
         <v>45</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>89</v>
+        <v>264</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="51" x14ac:dyDescent="0.25">
@@ -1987,13 +1986,13 @@
         <v>45</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>96</v>
+        <v>265</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -2004,24 +2003,30 @@
         <v>45</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>96</v>
+        <v>265</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
+      <c r="A42" s="6">
+        <v>6</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>265</v>
+      </c>
       <c r="D42" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
@@ -2032,13 +2037,13 @@
         <v>45</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>97</v>
+        <v>266</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2049,13 +2054,13 @@
         <v>45</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>96</v>
+        <v>265</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -2066,13 +2071,13 @@
         <v>45</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>96</v>
+        <v>265</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2089,7 +2094,7 @@
         <v>47</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2106,7 +2111,7 @@
         <v>48</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -2123,7 +2128,7 @@
         <v>50</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2140,7 +2145,7 @@
         <v>51</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2157,7 +2162,7 @@
         <v>52</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2174,7 +2179,7 @@
         <v>53</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -2191,7 +2196,7 @@
         <v>49</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2208,7 +2213,7 @@
         <v>54</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2225,7 +2230,7 @@
         <v>56</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2242,7 +2247,7 @@
         <v>57</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2259,7 +2264,7 @@
         <v>58</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2276,7 +2281,7 @@
         <v>55</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2293,7 +2298,7 @@
         <v>6.3</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
@@ -2310,7 +2315,7 @@
         <v>7.1</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2327,7 +2332,7 @@
         <v>63</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2344,7 +2349,7 @@
         <v>64</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2361,7 +2366,7 @@
         <v>65</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2378,7 +2383,7 @@
         <v>66</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2395,7 +2400,7 @@
         <v>68</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -2412,7 +2417,7 @@
         <v>69</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2429,7 +2434,7 @@
         <v>70</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2446,7 +2451,7 @@
         <v>72</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2463,7 +2468,7 @@
         <v>73</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2480,7 +2485,7 @@
         <v>74</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2497,7 +2502,7 @@
         <v>75</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2508,13 +2513,13 @@
         <v>60</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>98</v>
+        <v>267</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2525,13 +2530,13 @@
         <v>60</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>102</v>
+        <v>268</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2542,13 +2547,13 @@
         <v>60</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>102</v>
+        <v>268</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2559,13 +2564,13 @@
         <v>60</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>102</v>
+        <v>268</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2576,13 +2581,13 @@
         <v>60</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>109</v>
+        <v>269</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2593,13 +2598,13 @@
         <v>60</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>109</v>
+        <v>269</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2610,13 +2615,13 @@
         <v>60</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>109</v>
+        <v>269</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2627,13 +2632,13 @@
         <v>60</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>109</v>
+        <v>269</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2644,13 +2649,13 @@
         <v>60</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>109</v>
+        <v>269</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="51" x14ac:dyDescent="0.25">
@@ -2661,13 +2666,13 @@
         <v>60</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>109</v>
+        <v>269</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="51" x14ac:dyDescent="0.25">
@@ -2675,16 +2680,16 @@
         <v>8</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2692,16 +2697,16 @@
         <v>8</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2709,16 +2714,16 @@
         <v>8</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -2726,16 +2731,16 @@
         <v>8</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D84" s="6">
         <v>8.1999999999999993</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2743,16 +2748,16 @@
         <v>8</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D85" s="6">
         <v>8.3000000000000007</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2760,16 +2765,16 @@
         <v>9</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -2777,16 +2782,16 @@
         <v>9</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2794,16 +2799,16 @@
         <v>9</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2811,16 +2816,16 @@
         <v>9</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2828,16 +2833,16 @@
         <v>9</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2845,16 +2850,16 @@
         <v>9</v>
       </c>
       <c r="B91" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D91" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C91" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="E91" s="7" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2862,16 +2867,16 @@
         <v>9</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2879,16 +2884,16 @@
         <v>9</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>128</v>
+        <v>270</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2896,16 +2901,16 @@
         <v>9</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>128</v>
+        <v>270</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2913,16 +2918,16 @@
         <v>9</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>128</v>
+        <v>270</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="51" x14ac:dyDescent="0.25">
@@ -2930,16 +2935,16 @@
         <v>9</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>129</v>
+        <v>271</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2947,16 +2952,16 @@
         <v>9</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>129</v>
+        <v>271</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -2964,16 +2969,16 @@
         <v>9</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>129</v>
+        <v>271</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2981,16 +2986,16 @@
         <v>9</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>133</v>
+        <v>272</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -2998,16 +3003,16 @@
         <v>9</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>134</v>
+        <v>273</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -3015,16 +3020,16 @@
         <v>9</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>134</v>
+        <v>273</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -3032,16 +3037,16 @@
         <v>9</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>134</v>
+        <v>273</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -3049,16 +3054,16 @@
         <v>9</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>134</v>
+        <v>273</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -3066,16 +3071,16 @@
         <v>9</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>134</v>
+        <v>273</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -3083,16 +3088,16 @@
         <v>9</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>134</v>
+        <v>273</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -3100,16 +3105,16 @@
         <v>9</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>134</v>
+        <v>273</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3117,16 +3122,16 @@
         <v>9</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>134</v>
+        <v>273</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -3134,16 +3139,16 @@
         <v>9</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>134</v>
+        <v>273</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3151,16 +3156,16 @@
         <v>9</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>134</v>
+        <v>273</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -3168,16 +3173,16 @@
         <v>9</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>145</v>
+        <v>274</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -3185,16 +3190,16 @@
         <v>10</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D111" s="6">
         <v>10.1</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -3202,16 +3207,16 @@
         <v>10</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3219,16 +3224,16 @@
         <v>10</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -3236,16 +3241,16 @@
         <v>10</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -3253,16 +3258,16 @@
         <v>10</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
@@ -3270,16 +3275,16 @@
         <v>10</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3287,16 +3292,16 @@
         <v>10</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3304,16 +3309,16 @@
         <v>10</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="E118" s="7" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -3321,16 +3326,16 @@
         <v>10</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -3338,16 +3343,16 @@
         <v>10</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3355,16 +3360,16 @@
         <v>10</v>
       </c>
       <c r="B121" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D121" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C121" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="D121" s="6" t="s">
-        <v>158</v>
-      </c>
       <c r="E121" s="7" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uploading assets by excel file
</commit_message>
<xml_diff>
--- a/Audit_Code/public/ISO_SEC_2_2.xlsx
+++ b/Audit_Code/public/ISO_SEC_2_2.xlsx
@@ -1307,8 +1307,8 @@
   <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C110" sqref="C110"/>
+      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>